<commit_message>
Fixing cell format in Wood furnaces
</commit_message>
<xml_diff>
--- a/inst/extdata/Machines - Data/Wood furnaces/Wood furnaces.xlsx
+++ b/inst/extdata/Machines - Data/Wood furnaces/Wood furnaces.xlsx
@@ -162,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -177,6 +177,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -514,7 +517,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,10 +619,10 @@
       <c r="G4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="8">
         <v>1.6770082173402701E-2</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="8">
         <v>1.6770082173402701E-2</v>
       </c>
     </row>

</xml_diff>